<commit_message>
Read Excel File using pyExcel
</commit_message>
<xml_diff>
--- a/activeContact.xlsx
+++ b/activeContact.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>supportId</t>
-  </si>
-  <si>
     <t>customerName</t>
   </si>
   <si>
@@ -34,16 +31,45 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>icn</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>janedoe@acme.com</t>
+  </si>
+  <si>
+    <t>joshsmith@jones.com</t>
+  </si>
+  <si>
+    <t>teddybear@price.com</t>
+  </si>
+  <si>
+    <t>afisher@kmart.com</t>
+  </si>
+  <si>
+    <t>Kmart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,14 +92,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -373,63 +402,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>200300</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>400</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
+        <v>200</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>300</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>